<commit_message>
Adjust PPI demo 5 file for documentation download
</commit_message>
<xml_diff>
--- a/test-files/demo-files/18_proteins_81_edges_PPI.xlsx
+++ b/test-files/demo-files/18_proteins_81_edges_PPI.xlsx
@@ -1,89 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kdahlqui\Documents\GRNsight\PPI\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71A36FB1-688C-40DD-BF65-0094BC32FA39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <workbookPr date1904="false"/>
   <sheets>
     <sheet name="network" sheetId="1" r:id="rId1"/>
+    <sheet name="optimization_parameters" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="19">
-  <si>
-    <t>Aim32p</t>
-  </si>
-  <si>
-    <t>Ccr4p</t>
-  </si>
-  <si>
-    <t>Erv1p</t>
-  </si>
-  <si>
-    <t>Fbp1p</t>
-  </si>
-  <si>
-    <t>Hsc82p</t>
-  </si>
-  <si>
-    <t>Hsp78p</t>
-  </si>
-  <si>
-    <t>Mia40p</t>
-  </si>
-  <si>
-    <t>Mpt5p</t>
-  </si>
-  <si>
-    <t>Nab2p</t>
-  </si>
-  <si>
-    <t>Osm1p</t>
-  </si>
-  <si>
-    <t>Puf3p</t>
-  </si>
-  <si>
-    <t>Sod2p</t>
-  </si>
-  <si>
-    <t>Srp54p</t>
-  </si>
-  <si>
-    <t>Ssc1p</t>
-  </si>
-  <si>
-    <t>Tim17p</t>
-  </si>
-  <si>
-    <t>Tim22p</t>
-  </si>
-  <si>
-    <t>Tim23p</t>
-  </si>
-  <si>
-    <t>Tim50p</t>
-  </si>
-  <si>
-    <t>protein 1/protein 2</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
+  <fonts count="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -113,21 +41,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -452,77 +372,71 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:S19"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" t="s">
-        <v>16</v>
-      </c>
-      <c r="S1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>cols protein1/ rows protein2</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Aim32p</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Ccr4p</v>
+      </c>
+      <c r="D1" t="str">
+        <v>Erv1p</v>
+      </c>
+      <c r="E1" t="str">
+        <v>Fbp1p</v>
+      </c>
+      <c r="F1" t="str">
+        <v>Hsc82p</v>
+      </c>
+      <c r="G1" t="str">
+        <v>Hsp78p</v>
+      </c>
+      <c r="H1" t="str">
+        <v>Mia40p</v>
+      </c>
+      <c r="I1" t="str">
+        <v>Mpt5p</v>
+      </c>
+      <c r="J1" t="str">
+        <v>Nab2p</v>
+      </c>
+      <c r="K1" t="str">
+        <v>Osm1p</v>
+      </c>
+      <c r="L1" t="str">
+        <v>Puf3p</v>
+      </c>
+      <c r="M1" t="str">
+        <v>Sod2p</v>
+      </c>
+      <c r="N1" t="str">
+        <v>Srp54p</v>
+      </c>
+      <c r="O1" t="str">
+        <v>Ssc1p</v>
+      </c>
+      <c r="P1" t="str">
+        <v>Tim17p</v>
+      </c>
+      <c r="Q1" t="str">
+        <v>Tim22p</v>
+      </c>
+      <c r="R1" t="str">
+        <v>Tim23p</v>
+      </c>
+      <c r="S1" t="str">
+        <v>Tim50p</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>Aim32p</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -579,9 +493,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1</v>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>Ccr4p</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -638,9 +552,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>Erv1p</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -697,9 +611,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3</v>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>Fbp1p</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -756,9 +670,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>4</v>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>Hsc82p</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -815,9 +729,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>5</v>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>Hsp78p</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -874,9 +788,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>6</v>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>Mia40p</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -933,9 +847,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>7</v>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>Mpt5p</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -992,9 +906,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>8</v>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>Nab2p</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -1051,9 +965,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>9</v>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>Osm1p</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -1110,9 +1024,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>10</v>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>Puf3p</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -1169,9 +1083,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>11</v>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>Sod2p</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -1228,9 +1142,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>12</v>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>Srp54p</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -1287,9 +1201,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>13</v>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>Ssc1p</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -1346,9 +1260,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>14</v>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>Tim17p</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -1405,9 +1319,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>15</v>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>Tim22p</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -1464,9 +1378,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>16</v>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>Tim23p</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -1523,9 +1437,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>17</v>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>Tim50p</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -1583,6 +1497,45 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B4"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>optimization_parameter</v>
+      </c>
+      <c r="B1" t="str">
+        <v>value</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>species</v>
+      </c>
+      <c r="B2" t="str">
+        <v>Saccharomyces cerevisiae</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>taxon_id</v>
+      </c>
+      <c r="B3">
+        <v>559292</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>workbookType</v>
+      </c>
+      <c r="B4" t="str">
+        <v>protein-protein-physical-interaction</v>
+      </c>
+    </row>
+  </sheetData>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Modify demo 5 PPI files to be consistent with main
</commit_message>
<xml_diff>
--- a/test-files/demo-files/18_proteins_81_edges_PPI.xlsx
+++ b/test-files/demo-files/18_proteins_81_edges_PPI.xlsx
@@ -1,89 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kdahlqui\Documents\GRNsight\PPI\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71A36FB1-688C-40DD-BF65-0094BC32FA39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <workbookPr date1904="false"/>
   <sheets>
     <sheet name="network" sheetId="1" r:id="rId1"/>
+    <sheet name="optimization_parameters" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="19">
-  <si>
-    <t>Aim32p</t>
-  </si>
-  <si>
-    <t>Ccr4p</t>
-  </si>
-  <si>
-    <t>Erv1p</t>
-  </si>
-  <si>
-    <t>Fbp1p</t>
-  </si>
-  <si>
-    <t>Hsc82p</t>
-  </si>
-  <si>
-    <t>Hsp78p</t>
-  </si>
-  <si>
-    <t>Mia40p</t>
-  </si>
-  <si>
-    <t>Mpt5p</t>
-  </si>
-  <si>
-    <t>Nab2p</t>
-  </si>
-  <si>
-    <t>Osm1p</t>
-  </si>
-  <si>
-    <t>Puf3p</t>
-  </si>
-  <si>
-    <t>Sod2p</t>
-  </si>
-  <si>
-    <t>Srp54p</t>
-  </si>
-  <si>
-    <t>Ssc1p</t>
-  </si>
-  <si>
-    <t>Tim17p</t>
-  </si>
-  <si>
-    <t>Tim22p</t>
-  </si>
-  <si>
-    <t>Tim23p</t>
-  </si>
-  <si>
-    <t>Tim50p</t>
-  </si>
-  <si>
-    <t>protein 1/protein 2</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
+  <fonts count="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -113,21 +41,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -452,77 +372,71 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:S19"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" t="s">
-        <v>16</v>
-      </c>
-      <c r="S1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>cols protein1/ rows protein2</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Aim32p</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Ccr4p</v>
+      </c>
+      <c r="D1" t="str">
+        <v>Erv1p</v>
+      </c>
+      <c r="E1" t="str">
+        <v>Fbp1p</v>
+      </c>
+      <c r="F1" t="str">
+        <v>Hsc82p</v>
+      </c>
+      <c r="G1" t="str">
+        <v>Hsp78p</v>
+      </c>
+      <c r="H1" t="str">
+        <v>Mia40p</v>
+      </c>
+      <c r="I1" t="str">
+        <v>Mpt5p</v>
+      </c>
+      <c r="J1" t="str">
+        <v>Nab2p</v>
+      </c>
+      <c r="K1" t="str">
+        <v>Osm1p</v>
+      </c>
+      <c r="L1" t="str">
+        <v>Puf3p</v>
+      </c>
+      <c r="M1" t="str">
+        <v>Sod2p</v>
+      </c>
+      <c r="N1" t="str">
+        <v>Srp54p</v>
+      </c>
+      <c r="O1" t="str">
+        <v>Ssc1p</v>
+      </c>
+      <c r="P1" t="str">
+        <v>Tim17p</v>
+      </c>
+      <c r="Q1" t="str">
+        <v>Tim22p</v>
+      </c>
+      <c r="R1" t="str">
+        <v>Tim23p</v>
+      </c>
+      <c r="S1" t="str">
+        <v>Tim50p</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>Aim32p</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -579,9 +493,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1</v>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>Ccr4p</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -638,9 +552,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>Erv1p</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -697,9 +611,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3</v>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>Fbp1p</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -756,9 +670,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>4</v>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>Hsc82p</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -815,9 +729,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>5</v>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>Hsp78p</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -874,9 +788,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>6</v>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>Mia40p</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -933,9 +847,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>7</v>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>Mpt5p</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -992,9 +906,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>8</v>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>Nab2p</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -1051,9 +965,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>9</v>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>Osm1p</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -1110,9 +1024,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>10</v>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>Puf3p</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -1169,9 +1083,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>11</v>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>Sod2p</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -1228,9 +1142,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>12</v>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>Srp54p</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -1287,9 +1201,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>13</v>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>Ssc1p</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -1346,9 +1260,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>14</v>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>Tim17p</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -1405,9 +1319,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>15</v>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>Tim22p</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -1464,9 +1378,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>16</v>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>Tim23p</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -1523,9 +1437,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>17</v>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>Tim50p</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -1583,6 +1497,45 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B4"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>optimization_parameter</v>
+      </c>
+      <c r="B1" t="str">
+        <v>value</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>species</v>
+      </c>
+      <c r="B2" t="str">
+        <v>Saccharomyces cerevisiae</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>taxon_id</v>
+      </c>
+      <c r="B3">
+        <v>559292</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>workbookType</v>
+      </c>
+      <c r="B4" t="str">
+        <v>protein-protein-physical-interaction</v>
+      </c>
+    </row>
+  </sheetData>
 </worksheet>
 </file>
</xml_diff>